<commit_message>
moved b64 images to constants file
</commit_message>
<xml_diff>
--- a/test_scripts/chrome/QS002_testscript.xlsx
+++ b/test_scripts/chrome/QS002_testscript.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\edge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803BF924-29FD-4749-89AC-BDE27AA49165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC35ED84-1DFA-4934-AE47-11CA71180858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
+    <workbookView xWindow="3972" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>htatras2_dragable_css;htatras_droppable_css</t>
   </si>
   <si>
-    <t>htat2;droppable area</t>
-  </si>
-  <si>
     <t>htatras1_dragable_css;htatras_droppable_css</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>wait_for_seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">htat2; </t>
   </si>
 </sst>
 </file>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3916CC0C-2E25-4DCF-A97F-45AF0FE46343}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -668,7 +668,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -690,12 +690,12 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -706,15 +706,15 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -725,10 +725,10 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>